<commit_message>
feat: allow admin to edit any user's entry and add username field in edit form
</commit_message>
<xml_diff>
--- a/foaie_parcurs.xlsx
+++ b/foaie_parcurs.xlsx
@@ -468,16 +468,16 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Zona 2</t>
+          <t>Zona 5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Client Z2-1</t>
+          <t>Potentiali clienti noi</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
feat: improve login and registration form styling
</commit_message>
<xml_diff>
--- a/foaie_parcurs.xlsx
+++ b/foaie_parcurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,20 +468,120 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>Zona 4</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CORONITAS SERVCOM SRL</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ioana</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Zona 3</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>DEDEMAN</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>andrei</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Zona 4</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AGROLIV SRL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>7</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>andrei</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>Zona 5</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Potentiali clienti noi</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>6</v>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>EUROCONSTRUCT SRL COVASNA</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>100</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>2025-08-11</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>ioana</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Zona 4</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MACON SRL BISTRITA</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>677</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>2025-08-06</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: reversed database query ordering on index page
</commit_message>
<xml_diff>
--- a/foaie_parcurs.xlsx
+++ b/foaie_parcurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,11 +473,11 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CORONITAS SERVCOM SRL</t>
+          <t>CRISTAL TURISM SRL</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -582,6 +582,81 @@
       <c r="E6" t="inlineStr">
         <is>
           <t>2025-08-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Zona 3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>DEDEMAN</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>344</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>2025-08-01</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Zona 4</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>VIAMSO SRL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>100</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Zona 2</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>ARTHA STRUCTURE AG S.R.L</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>567</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: enhance edit page UI for phone use
</commit_message>
<xml_diff>
--- a/foaie_parcurs.xlsx
+++ b/foaie_parcurs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,6 +660,106 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Zona 3</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BOB TRADING SRL</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>53</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Zona 5</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BONA LUX CENTER S.R.L.</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>694</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Zona 3</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>MARCO CHIM SRL</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>6435</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>maria.ioana.dicu@gmail.com</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Zona 3</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Administrativ</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>54</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2025-08-12</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>